<commit_message>
PWR UPDATES - Update SNSP 2030 limit to 70% - Update PWR Dispatchable Plants Efficiencies - ADD GAS CCS Start date option of 2027 as per ERVIVA PLANS - ADD BECCS Start date option of 2027 - ADD CCS 97% capture rate option
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_PWR_SNSP.xlsx
+++ b/SuppXLS/Scen_PWR_SNSP.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olex\Documents\MANRID\ResLab\Modelling\TIMES\TIMES-IE\SuppXLS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\VEDA\VEDA_Models\~g2v_TIMES-Ireland-model\main\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB4D05DE-34DD-438E-B7B0-708A7582BB95}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0299A1B5-228F-4E0E-B371-BB2FE058998F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-3233" yWindow="8002" windowWidth="20716" windowHeight="13276" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="13110" yWindow="6525" windowWidth="28110" windowHeight="15990" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Regions" sheetId="2" r:id="rId1"/>
@@ -1738,8 +1738,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:T14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="N9" sqref="N9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1897,7 +1897,7 @@
         <v>0</v>
       </c>
       <c r="N8" s="14">
-        <v>-0.75</v>
+        <v>-0.7</v>
       </c>
       <c r="O8" s="12">
         <v>0</v>
@@ -1939,7 +1939,7 @@
       <c r="M9" s="12"/>
       <c r="N9" s="14">
         <f>1+N8</f>
-        <v>0.25</v>
+        <v>0.30000000000000004</v>
       </c>
       <c r="P9" s="14">
         <f>1+P8</f>

</xml_diff>